<commit_message>
Fixed column headers from new files using the old headers from a parallel branch.
Files checked in: DataRepo/data/tests/multiple_representations/resolution_handling/prereqs.xlsx
</commit_message>
<xml_diff>
--- a/DataRepo/data/tests/multiple_representations/resolution_handling/prereqs.xlsx
+++ b/DataRepo/data/tests/multiple_representations/resolution_handling/prereqs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-LOCAL/TRACEBASE/tracebase/DataRepo/data/tests/multiple_representations/conflicting_resolutions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-LOCAL/TRACEBASE/tracebase/DataRepo/data/tests/multiple_representations/resolution_handling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0884DB85-3495-D74B-9630-6C579B0234CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B78F69F-F02E-F549-8F95-6BB660ABAF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="500" windowWidth="37400" windowHeight="20800" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="400" yWindow="500" windowWidth="37400" windowHeight="20800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -1849,7 +1849,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -1959,9 +1959,6 @@
     <t>Tracer Row Group</t>
   </si>
   <si>
-    <t>Compound Name</t>
-  </si>
-  <si>
     <t>Mass Number</t>
   </si>
   <si>
@@ -2083,6 +2080,12 @@
   </si>
   <si>
     <t>Exploris240</t>
+  </si>
+  <si>
+    <t>Tracer</t>
+  </si>
+  <si>
+    <t>Sequence</t>
   </si>
 </sst>
 </file>
@@ -3372,10 +3375,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3410,44 +3413,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>73</v>
-      </c>
-      <c r="D2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
         <v>75</v>
       </c>
-      <c r="C3" t="s">
-        <v>76</v>
-      </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3485,10 +3488,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -3496,16 +3499,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
         <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
       </c>
       <c r="C2">
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3720,34 +3723,34 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2">
         <v>12</v>
       </c>
       <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
         <v>57</v>
-      </c>
-      <c r="D2" t="s">
-        <v>58</v>
       </c>
       <c r="E2">
         <v>30.5</v>
       </c>
       <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
         <v>62</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>63</v>
       </c>
-      <c r="I2" t="s">
-        <v>64</v>
-      </c>
       <c r="J2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3867,22 +3870,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3">
         <v>45356</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3923,7 +3926,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3948,7 +3953,7 @@
         <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>24</v>
@@ -3956,30 +3961,30 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" t="s">
-        <v>67</v>
-      </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
         <v>68</v>
-      </c>
-      <c r="E3" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -4014,7 +4019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4052,13 +4057,13 @@
         <v>Michael Neinast, polar-HILIC-25-min, Exploris240, 2024-03-08</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E2" s="3">
         <v>45359</v>
@@ -4163,7 +4168,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4182,7 +4189,7 @@
         <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -4196,7 +4203,7 @@
         <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2">
         <v>7000</v>
@@ -4367,7 +4374,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4385,19 +4394,19 @@
         <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>32</v>
@@ -4408,13 +4417,13 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -4590,18 +4599,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -4642,10 +4651,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>